<commit_message>
Created new code for AD
</commit_message>
<xml_diff>
--- a/AWS-SSO-Integrate-with_Azure_AD/Roles_Name.xlsx
+++ b/AWS-SSO-Integrate-with_Azure_AD/Roles_Name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jetstarairways-my.sharepoint.com/personal/balraj_singh_jetstar_com/Documents/Balraj_D_Laptop_Drive/DevOps_Master/Azure_DevOps_Projects/AWS-SSO-Integrate-with_Azure_AD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{6FFE23F1-3CB7-4180-BA9C-C8878493D991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5728FB5C-16B9-465F-A8BE-8DE288D58E55}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{6FFE23F1-3CB7-4180-BA9C-C8878493D991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CA5B5DD-438B-4DDE-A5D5-1DA2A781BCF5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="960" windowWidth="20640" windowHeight="11160" xr2:uid="{8E22F0A2-2342-422B-BB0D-4C89B0B550B6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E22F0A2-2342-422B-BB0D-4C89B0B550B6}"/>
   </bookViews>
   <sheets>
     <sheet name="AWS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ARN</t>
   </si>
@@ -47,9 +47,6 @@
     <t>AD Users</t>
   </si>
   <si>
-    <t>Azure AD</t>
-  </si>
-  <si>
     <t>AWS-User-Admin</t>
   </si>
   <si>
@@ -99,6 +96,15 @@
   </si>
   <si>
     <t>Nil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18th </t>
+  </si>
+  <si>
+    <t>invocie- auto -dept</t>
+  </si>
+  <si>
+    <t>Azure AD Group</t>
   </si>
 </sst>
 </file>
@@ -145,7 +151,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F901A1B-1D06-41FB-9890-5AEC464235C4}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,6 +500,7 @@
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -499,13 +508,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -513,58 +522,66 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>